<commit_message>
update machinery info script
</commit_message>
<xml_diff>
--- a/DE/DE.xlsx
+++ b/DE/DE.xlsx
@@ -8,20 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32906c935fa0eb4f/models/DE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1860" documentId="8_{2959E65E-55D8-40F5-B350-6BD91C9C1EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F74DBC7-008A-4F6A-A0D7-F03D4FD796D7}"/>
+  <xr:revisionPtr revIDLastSave="1871" documentId="8_{2959E65E-55D8-40F5-B350-6BD91C9C1EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49F33FDD-F59E-4AE4-A280-933A0192F747}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="450" windowWidth="14170" windowHeight="9980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="430" yWindow="790" windowWidth="14170" windowHeight="9980" activeTab="2" xr2:uid="{218BED0F-FD75-4FFF-A66C-349F9BB7DC71}"/>
+    <workbookView xWindow="1450" yWindow="950" windowWidth="17580" windowHeight="19410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main" sheetId="1" r:id="rId1"/>
-    <sheet name="Model" sheetId="7" r:id="rId2"/>
-    <sheet name="Scripting" sheetId="8" r:id="rId3"/>
-    <sheet name="Parts" sheetId="5" r:id="rId4"/>
-    <sheet name="Notes" sheetId="6" r:id="rId5"/>
-    <sheet name="Manufacturing" sheetId="3" r:id="rId6"/>
-    <sheet name="ModelOLD" sheetId="2" r:id="rId7"/>
-    <sheet name="IP" sheetId="4" r:id="rId8"/>
+    <sheet name="main" sheetId="1" r:id="rId1"/>
+    <sheet name="model" sheetId="7" r:id="rId2"/>
+    <sheet name="parts" sheetId="5" r:id="rId3"/>
+    <sheet name="notes" sheetId="6" r:id="rId4"/>
+    <sheet name="Manufacturing" sheetId="3" r:id="rId5"/>
+    <sheet name="ModelOLD" sheetId="2" r:id="rId6"/>
+    <sheet name="IP" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="265">
   <si>
     <t>Price</t>
   </si>
@@ -856,9 +854,6 @@
     <t>Employees</t>
   </si>
   <si>
-    <t>Most Recent</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -869,6 +864,9 @@
   </si>
   <si>
     <t>xxx</t>
+  </si>
+  <si>
+    <t>use for scripting</t>
   </si>
 </sst>
 </file>
@@ -882,7 +880,7 @@
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1012,12 +1010,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1540,7 +1532,6 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
@@ -1737,12 +1728,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858921DB-62EE-49E5-94B1-0F56666D22CA}">
   <dimension ref="A1:XEY119"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I51" sqref="I51"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1755,13 +1743,34 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C1" t="s">
         <v>260</v>
       </c>
+      <c r="D1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G1" t="s">
+        <v>260</v>
+      </c>
+      <c r="H1" t="s">
+        <v>260</v>
+      </c>
       <c r="I1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J1" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
+      </c>
+      <c r="K1" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1772,12 +1781,12 @@
         <v>45229</v>
       </c>
       <c r="J2" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="47" customFormat="1">
       <c r="A3" s="47" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B3" s="47" t="s">
         <v>256</v>
@@ -1804,7 +1813,7 @@
         <v>53</v>
       </c>
       <c r="J3" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K3" s="47">
         <v>2023</v>
@@ -1815,7 +1824,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="J4" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="55" customFormat="1">
@@ -1826,7 +1835,7 @@
         <v>83000</v>
       </c>
       <c r="J5" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="55" customFormat="1">
@@ -1837,7 +1846,7 @@
         <v>2050</v>
       </c>
       <c r="J6" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="48" customFormat="1">
@@ -1851,7 +1860,7 @@
         <v>7900</v>
       </c>
       <c r="J7" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1868,7 +1877,7 @@
         <v>3300</v>
       </c>
       <c r="J8" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1885,17 +1894,17 @@
         <v>6400</v>
       </c>
       <c r="J9" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="J10" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C11" s="48">
         <v>5112</v>
@@ -1920,7 +1929,7 @@
         <v>5038</v>
       </c>
       <c r="J11" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K11" s="48">
         <v>26450</v>
@@ -1954,7 +1963,7 @@
         <v>2168</v>
       </c>
       <c r="J12" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K12" s="48">
         <v>10122</v>
@@ -1988,7 +1997,7 @@
         <v>825</v>
       </c>
       <c r="J13" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K13" s="48">
         <v>3505</v>
@@ -2022,7 +2031,7 @@
         <v>1308</v>
       </c>
       <c r="J14" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K14" s="48">
         <v>6842</v>
@@ -2056,7 +2065,7 @@
         <v>643</v>
       </c>
       <c r="J15" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K15" s="48">
         <v>2451</v>
@@ -2090,7 +2099,7 @@
         <v>961</v>
       </c>
       <c r="J16" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K16" s="48">
         <v>3794</v>
@@ -2124,7 +2133,7 @@
         <v>269</v>
       </c>
       <c r="J17" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K17" s="48">
         <v>1429</v>
@@ -2158,7 +2167,7 @@
         <v>1595</v>
       </c>
       <c r="J18" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K18" s="48">
         <v>5094</v>
@@ -2192,7 +2201,7 @@
         <v>345</v>
       </c>
       <c r="J19" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K19" s="48">
         <v>1564</v>
@@ -2232,7 +2241,7 @@
         <v>13152</v>
       </c>
       <c r="J20" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K20" s="49">
         <f>SUM(K11:K19)</f>
@@ -18619,7 +18628,7 @@
       <c r="H21" s="48"/>
       <c r="I21" s="48"/>
       <c r="J21" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="22" spans="1:16379">
@@ -18649,7 +18658,7 @@
         <v>7706</v>
       </c>
       <c r="J22" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K22" s="48">
         <v>34105</v>
@@ -18683,7 +18692,7 @@
         <v>1070</v>
       </c>
       <c r="J23" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K23" s="48">
         <v>4287</v>
@@ -18717,7 +18726,7 @@
         <v>1560</v>
       </c>
       <c r="J24" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K24" s="48">
         <v>7321</v>
@@ -18751,7 +18760,7 @@
         <v>389</v>
       </c>
       <c r="J25" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K25" s="48">
         <v>2137</v>
@@ -18785,7 +18794,7 @@
         <v>1365</v>
       </c>
       <c r="J26" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K26" s="48">
         <v>8197</v>
@@ -18819,7 +18828,7 @@
         <v>1062</v>
       </c>
       <c r="J27" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K27" s="48">
         <v>5204</v>
@@ -18859,7 +18868,7 @@
         <v>13152</v>
       </c>
       <c r="J28" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K28" s="49">
         <f>SUM(K22:K27)</f>
@@ -18872,7 +18881,7 @@
     </row>
     <row r="29" spans="1:16379">
       <c r="J29" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="30" spans="1:16379" s="47" customFormat="1">
@@ -18905,7 +18914,7 @@
         <v>Q324</v>
       </c>
       <c r="J30" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K30" s="47">
         <f t="shared" ref="K30:L30" si="6">K3</f>
@@ -18921,7 +18930,7 @@
         <v>159</v>
       </c>
       <c r="J31" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" spans="1:16379">
@@ -18950,7 +18959,7 @@
         <v>11387</v>
       </c>
       <c r="J32" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K32" s="48">
         <f>SUM(C32:F32)</f>
@@ -18987,7 +18996,7 @@
         <v>1461</v>
       </c>
       <c r="J33" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K33" s="48">
         <f>SUM(C33:F33)</f>
@@ -19024,7 +19033,7 @@
         <v>304</v>
       </c>
       <c r="J34" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K34" s="48">
         <f>SUM(C34:F34)</f>
@@ -19068,7 +19077,7 @@
         <v>13152</v>
       </c>
       <c r="J35" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K35" s="49">
         <f t="shared" ref="K35:L35" si="8">SUM(K32:K34)</f>
@@ -19105,7 +19114,7 @@
         <v>7848</v>
       </c>
       <c r="J36" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K36" s="48">
         <f>SUM(C36:F36)</f>
@@ -19149,7 +19158,7 @@
         <v>5304</v>
       </c>
       <c r="J37" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K37" s="49">
         <f t="shared" ref="K37:L37" si="10">K35-K36</f>
@@ -19186,7 +19195,7 @@
         <v>567</v>
       </c>
       <c r="J38" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K38" s="48">
         <f>SUM(C38:F38)</f>
@@ -19223,7 +19232,7 @@
         <v>1278</v>
       </c>
       <c r="J39" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K39" s="48">
         <f>SUM(C39:F39)</f>
@@ -19260,7 +19269,7 @@
         <v>840</v>
       </c>
       <c r="J40" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K40" s="48">
         <f>SUM(C40:F40)</f>
@@ -19297,7 +19306,7 @@
         <v>264</v>
       </c>
       <c r="J41" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K41" s="48">
         <f>SUM(C41:F41)</f>
@@ -19341,7 +19350,7 @@
         <v>10797</v>
       </c>
       <c r="J42" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K42" s="49">
         <f t="shared" ref="K42:L42" si="12">SUM(K38:K41)+K36</f>
@@ -19385,7 +19394,7 @@
         <v>2355</v>
       </c>
       <c r="J43" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K43" s="49">
         <f t="shared" ref="K43:L43" si="14">K35-K42</f>
@@ -19422,7 +19431,7 @@
         <v>625</v>
       </c>
       <c r="J44" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K44" s="48">
         <f>SUM(C44:F44)</f>
@@ -19466,7 +19475,7 @@
         <v>1730</v>
       </c>
       <c r="J45" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K45" s="49">
         <f t="shared" ref="K45:L45" si="16">K43-K44</f>
@@ -19503,7 +19512,7 @@
         <v>1</v>
       </c>
       <c r="J46" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K46" s="48">
         <f>SUM(C46:F46)</f>
@@ -19540,7 +19549,7 @@
         <v>-3</v>
       </c>
       <c r="J47" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K47" s="48">
         <f>SUM(C47:F47)</f>
@@ -19584,7 +19593,7 @@
         <v>1734</v>
       </c>
       <c r="J48" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K48" s="49">
         <f t="shared" ref="K48:L48" si="18">K45+K46-K47</f>
@@ -19597,7 +19606,7 @@
     </row>
     <row r="49" spans="1:12">
       <c r="J49" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="50" spans="1:12" s="47" customFormat="1">
@@ -19605,7 +19614,7 @@
         <v>182</v>
       </c>
       <c r="J50" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="51" spans="1:12" s="47" customFormat="1">
@@ -19641,7 +19650,7 @@
         <v>6.3169398907103824</v>
       </c>
       <c r="J51" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K51" s="53">
         <f t="shared" ref="K51:L51" si="20">K48/K57</f>
@@ -19685,7 +19694,7 @@
         <v>6.3146394756008739</v>
       </c>
       <c r="J52" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K52" s="53">
         <f t="shared" ref="K52:L52" si="22">K48/K58</f>
@@ -19722,7 +19731,7 @@
         <v>1.47</v>
       </c>
       <c r="J53" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K53" s="51">
         <f>SUM(C53:F53)</f>
@@ -19759,7 +19768,7 @@
         <v>1.47</v>
       </c>
       <c r="J54" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K54" s="51">
         <f>SUM(C54:F54)</f>
@@ -19779,7 +19788,7 @@
       <c r="H55" s="50"/>
       <c r="I55" s="50"/>
       <c r="J55" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="56" spans="1:12" s="47" customFormat="1">
@@ -19794,7 +19803,7 @@
       <c r="H56" s="52"/>
       <c r="I56" s="52"/>
       <c r="J56" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -19823,7 +19832,7 @@
         <v>274.5</v>
       </c>
       <c r="J57" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K57">
         <v>292.2</v>
@@ -19855,7 +19864,7 @@
         <v>274.60000000000002</v>
       </c>
       <c r="J58" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K58">
         <v>293.60000000000002</v>
@@ -19863,7 +19872,7 @@
     </row>
     <row r="59" spans="1:12">
       <c r="J59" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -19898,7 +19907,7 @@
         <v>1730</v>
       </c>
       <c r="J60" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K60" s="48">
         <v>10155</v>
@@ -19937,7 +19946,7 @@
         <v>91</v>
       </c>
       <c r="J61" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K61" s="48">
         <v>-16</v>
@@ -19976,7 +19985,7 @@
         <v>553</v>
       </c>
       <c r="J62" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K62" s="48">
         <v>2004</v>
@@ -20006,7 +20015,7 @@
         <v>53</v>
       </c>
       <c r="J63" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K63" s="48">
         <v>191</v>
@@ -20045,7 +20054,7 @@
         <v>55</v>
       </c>
       <c r="J64" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K64" s="48">
         <v>130</v>
@@ -20084,7 +20093,7 @@
         <v>-5</v>
       </c>
       <c r="J65" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K65" s="48">
         <v>-790</v>
@@ -20123,7 +20132,7 @@
         <v>23</v>
       </c>
       <c r="J66" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K66" s="48">
         <v>-4253</v>
@@ -20162,7 +20171,7 @@
         <v>643</v>
       </c>
       <c r="J67" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K67" s="48">
         <v>279</v>
@@ -20201,7 +20210,7 @@
         <v>285</v>
       </c>
       <c r="J68" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K68" s="48">
         <v>830</v>
@@ -20240,7 +20249,7 @@
         <v>60</v>
       </c>
       <c r="J69" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K69" s="48">
         <v>-23</v>
@@ -20279,7 +20288,7 @@
         <v>-38</v>
       </c>
       <c r="J70" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K70" s="48">
         <v>-170</v>
@@ -20318,7 +20327,7 @@
         <v>-255</v>
       </c>
       <c r="J71" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K71" s="48">
         <v>252</v>
@@ -20359,7 +20368,7 @@
         <v>3195</v>
       </c>
       <c r="J72" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K72" s="49">
         <f t="shared" ref="K72:L72" si="25">SUM(K60:K71)</f>
@@ -20373,7 +20382,7 @@
     <row r="73" spans="1:12">
       <c r="D73" s="48"/>
       <c r="J73" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="74" spans="1:12" s="47" customFormat="1">
@@ -20406,7 +20415,7 @@
         <v>Q324</v>
       </c>
       <c r="J74" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K74" s="47">
         <f>K30</f>
@@ -20422,7 +20431,7 @@
         <v>24</v>
       </c>
       <c r="J75" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -20451,7 +20460,7 @@
         <v>7004</v>
       </c>
       <c r="J76" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K76" s="48">
         <f t="shared" ref="K76:K83" si="28">F76</f>
@@ -20484,7 +20493,7 @@
         <v>1140</v>
       </c>
       <c r="J77" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K77" s="48">
         <f t="shared" si="28"/>
@@ -20517,7 +20526,7 @@
         <v>7469</v>
       </c>
       <c r="J78" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K78" s="48">
         <f t="shared" si="28"/>
@@ -20550,7 +20559,7 @@
         <v>43896</v>
       </c>
       <c r="J79" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K79" s="48">
         <f t="shared" si="28"/>
@@ -20583,7 +20592,7 @@
         <v>8274</v>
       </c>
       <c r="J80" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K80" s="48">
         <f t="shared" si="28"/>
@@ -20616,7 +20625,7 @@
         <v>2270</v>
       </c>
       <c r="J81" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K81" s="48">
         <f t="shared" si="28"/>
@@ -20649,7 +20658,7 @@
         <v>7118</v>
       </c>
       <c r="J82" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K82" s="48">
         <f t="shared" si="28"/>
@@ -20682,7 +20691,7 @@
         <v>7696</v>
       </c>
       <c r="J83" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K83" s="48">
         <f t="shared" si="28"/>
@@ -20722,7 +20731,7 @@
         <v>84867</v>
       </c>
       <c r="J84" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K84" s="49">
         <f>SUM(K75:K83)</f>
@@ -20755,7 +20764,7 @@
         <v>7092</v>
       </c>
       <c r="J85" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K85" s="48">
         <f t="shared" ref="K85:K91" si="30">F85</f>
@@ -20788,7 +20797,7 @@
         <v>3960</v>
       </c>
       <c r="J86" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K86" s="48">
         <f t="shared" si="30"/>
@@ -20821,7 +20830,7 @@
         <v>1030</v>
       </c>
       <c r="J87" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K87" s="48">
         <f t="shared" si="30"/>
@@ -20854,7 +20863,7 @@
         <v>3126</v>
       </c>
       <c r="J88" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K88" s="48">
         <f t="shared" si="30"/>
@@ -20887,7 +20896,7 @@
         <v>1898</v>
       </c>
       <c r="J89" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K89" s="48">
         <f t="shared" si="30"/>
@@ -20920,7 +20929,7 @@
         <v>2903</v>
       </c>
       <c r="J90" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K90" s="48">
         <f t="shared" si="30"/>
@@ -20953,7 +20962,7 @@
         <v>2965</v>
       </c>
       <c r="J91" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K91" s="48">
         <f t="shared" si="30"/>
@@ -20993,7 +21002,7 @@
         <v>107841</v>
       </c>
       <c r="J92" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K92" s="49">
         <f t="shared" ref="K92" si="32">SUM(K84:K91)</f>
@@ -21002,7 +21011,7 @@
     </row>
     <row r="93" spans="1:11">
       <c r="J93" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="94" spans="1:11" s="47" customFormat="1">
@@ -21010,7 +21019,7 @@
         <v>203</v>
       </c>
       <c r="J94" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="95" spans="1:11">
@@ -21039,7 +21048,7 @@
         <v>15294</v>
       </c>
       <c r="J95" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K95" s="48">
         <f>F95</f>
@@ -21072,7 +21081,7 @@
         <v>7869</v>
       </c>
       <c r="J96" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K96" s="48">
         <f>F96</f>
@@ -21105,7 +21114,7 @@
         <v>14397</v>
       </c>
       <c r="J97" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K97" s="48">
         <f>F97</f>
@@ -21138,7 +21147,7 @@
         <v>481</v>
       </c>
       <c r="J98" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K98" s="48">
         <f>F98</f>
@@ -21178,7 +21187,7 @@
         <v>38041</v>
       </c>
       <c r="J99" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K99" s="49">
         <f>SUM(K95:K98)</f>
@@ -21211,7 +21220,7 @@
         <v>42692</v>
       </c>
       <c r="J100" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K100" s="48">
         <f>F100</f>
@@ -21244,7 +21253,7 @@
         <v>2156</v>
       </c>
       <c r="J101" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K101" s="48">
         <f>F101</f>
@@ -21277,7 +21286,7 @@
         <v>1803</v>
       </c>
       <c r="J102" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K102" s="48">
         <f>F102</f>
@@ -21317,7 +21326,7 @@
         <v>84692</v>
       </c>
       <c r="J103" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K103" s="49">
         <f>SUM(K99:K102)</f>
@@ -21350,7 +21359,7 @@
         <v>84</v>
       </c>
       <c r="J104" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K104" s="48">
         <f>F104</f>
@@ -21359,7 +21368,7 @@
     </row>
     <row r="105" spans="1:11">
       <c r="J105" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K105" s="48">
         <f>F105</f>
@@ -21399,7 +21408,7 @@
         <v>19311</v>
       </c>
       <c r="J106" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K106" s="49">
         <f>P92-K103-K104</f>
@@ -21411,7 +21420,7 @@
         <v>213</v>
       </c>
       <c r="J107" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="108" spans="1:11" s="48" customFormat="1">
@@ -21441,7 +21450,7 @@
         <v>5441</v>
       </c>
       <c r="J108" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K108" s="48">
         <f>F108</f>
@@ -21475,7 +21484,7 @@
         <v>-34570</v>
       </c>
       <c r="J109" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K109" s="48">
         <f>F109</f>
@@ -21509,7 +21518,7 @@
         <v>55559</v>
       </c>
       <c r="J110" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K110" s="48">
         <f>F110</f>
@@ -21543,7 +21552,7 @@
         <v>-3368</v>
       </c>
       <c r="J111" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K111" s="48">
         <f>F111</f>
@@ -21584,7 +21593,7 @@
         <v>23062</v>
       </c>
       <c r="J112" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K112" s="49">
         <f>SUM(K108:K111)</f>
@@ -21618,7 +21627,7 @@
         <v>3</v>
       </c>
       <c r="J113" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K113" s="48">
         <f>F113</f>
@@ -21659,7 +21668,7 @@
         <v>23065</v>
       </c>
       <c r="J114" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K114" s="49">
         <f>K113+K112</f>
@@ -21699,7 +21708,7 @@
         <v>107841</v>
       </c>
       <c r="J115" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K115" s="49">
         <f t="shared" ref="K115" si="39">K114+K103+K104</f>
@@ -21708,7 +21717,7 @@
     </row>
     <row r="116" spans="1:11">
       <c r="J116" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="117" spans="1:11" s="47" customFormat="1">
@@ -21744,7 +21753,7 @@
         <v>0.7853413822201204</v>
       </c>
       <c r="J117" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K117" s="52">
         <f t="shared" ref="K117" si="41">K103/K92</f>
@@ -21784,7 +21793,7 @@
         <v>2.2309350437685653</v>
       </c>
       <c r="J118" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K118" s="52">
         <f>K84/K99</f>
@@ -21824,7 +21833,7 @@
         <v>46826</v>
       </c>
       <c r="J119" s="56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K119" s="49">
         <f>K84-K99</f>
@@ -21838,205 +21847,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16C8C3E-949C-4F93-B195-32AB2E84ED27}">
-  <dimension ref="A1:H5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="J1" sqref="I1:J1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="27.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="str">
-        <f>Model!A3</f>
-        <v>Quarters</v>
-      </c>
-      <c r="B1" t="str">
-        <f>Model!C3</f>
-        <v>Q123</v>
-      </c>
-      <c r="C1" t="str">
-        <f>Model!D3</f>
-        <v>Q223</v>
-      </c>
-      <c r="D1" t="str">
-        <f>Model!E3</f>
-        <v>Q323</v>
-      </c>
-      <c r="E1" t="str">
-        <f>Model!F3</f>
-        <v>Q423</v>
-      </c>
-      <c r="F1" t="str">
-        <f>Model!G3</f>
-        <v>Q124</v>
-      </c>
-      <c r="G1" t="str">
-        <f>Model!H3</f>
-        <v>Q224</v>
-      </c>
-      <c r="H1" t="str">
-        <f>Model!I3</f>
-        <v>Q324</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="str">
-        <f>Model!A11</f>
-        <v>Production &amp; Precision Ag Sales</v>
-      </c>
-      <c r="B2">
-        <f>Model!C11</f>
-        <v>5112</v>
-      </c>
-      <c r="C2">
-        <f>Model!D11</f>
-        <v>7733</v>
-      </c>
-      <c r="D2">
-        <f>Model!E11</f>
-        <v>6721</v>
-      </c>
-      <c r="E2">
-        <f>Model!F11</f>
-        <v>6884</v>
-      </c>
-      <c r="F2">
-        <f>Model!G11</f>
-        <v>4791</v>
-      </c>
-      <c r="G2">
-        <f>Model!H11</f>
-        <v>6507</v>
-      </c>
-      <c r="H2">
-        <f>Model!I11</f>
-        <v>5038</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="str">
-        <f>Model!A32</f>
-        <v>Net Sales</v>
-      </c>
-      <c r="B3">
-        <f>Model!C32</f>
-        <v>11402</v>
-      </c>
-      <c r="C3">
-        <f>Model!D32</f>
-        <v>16079</v>
-      </c>
-      <c r="D3">
-        <f>Model!E32</f>
-        <v>14284</v>
-      </c>
-      <c r="E3">
-        <f>Model!F32</f>
-        <v>13801</v>
-      </c>
-      <c r="F3">
-        <f>Model!G32</f>
-        <v>10486</v>
-      </c>
-      <c r="G3">
-        <f>Model!H32</f>
-        <v>13610</v>
-      </c>
-      <c r="H3">
-        <f>Model!I32</f>
-        <v>11387</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="str">
-        <f>Model!A37</f>
-        <v>GM</v>
-      </c>
-      <c r="B4">
-        <f>Model!C37</f>
-        <v>4718</v>
-      </c>
-      <c r="C4">
-        <f>Model!D37</f>
-        <v>6657</v>
-      </c>
-      <c r="D4">
-        <f>Model!E37</f>
-        <v>6177</v>
-      </c>
-      <c r="E4">
-        <f>Model!F37</f>
-        <v>5985</v>
-      </c>
-      <c r="F4">
-        <f>Model!G37</f>
-        <v>4985</v>
-      </c>
-      <c r="G4">
-        <f>Model!H37</f>
-        <v>6078</v>
-      </c>
-      <c r="H4">
-        <f>Model!I37</f>
-        <v>5304</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="str">
-        <f>Model!A38</f>
-        <v>R&amp;D</v>
-      </c>
-      <c r="B5">
-        <f>Model!C38</f>
-        <v>495</v>
-      </c>
-      <c r="C5">
-        <f>Model!D38</f>
-        <v>547</v>
-      </c>
-      <c r="D5">
-        <f>Model!E38</f>
-        <v>528</v>
-      </c>
-      <c r="E5">
-        <f>Model!F38</f>
-        <v>606</v>
-      </c>
-      <c r="F5">
-        <f>Model!G38</f>
-        <v>533</v>
-      </c>
-      <c r="G5">
-        <f>Model!H38</f>
-        <v>565</v>
-      </c>
-      <c r="H5">
-        <f>Model!I38</f>
-        <v>567</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="20" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F884044-8D53-4D69-86C1-ADAE3CA21267}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -22296,14 +22112,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF238C3A-91E4-4025-92B8-65E0C240F210}">
   <dimension ref="B2:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -22497,14 +22312,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93975FF4-BC21-4380-828B-9AD627B5D152}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
@@ -22633,7 +22447,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E310252-7C49-48D8-9A64-7380C8DB275B}">
   <dimension ref="A1:AI114"/>
   <sheetViews>
@@ -22643,7 +22457,6 @@
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="F84" sqref="F84"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
@@ -25031,7 +24844,7 @@
         <v>48</v>
       </c>
       <c r="AG58" s="3" t="e">
-        <f>NPV(AG57,#REF!)+Main!K5-Main!K6</f>
+        <f>NPV(AG57,#REF!)+main!K5-main!K6</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -25418,7 +25231,7 @@
         <v>49</v>
       </c>
       <c r="AG75" s="10" t="e">
-        <f>AG58/Main!K3</f>
+        <f>AG58/main!K3</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -26467,14 +26280,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F181E2A2-167A-4FDD-9F1F-646C0DABC3EE}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>

</xml_diff>